<commit_message>
Add SmartLED Shield for Teensy 4 Hardware Files
</commit_message>
<xml_diff>
--- a/extras/hardware/SmartLEDShield_Teensy4_V0_BOM.xlsx
+++ b/extras/hardware/SmartLEDShield_Teensy4_V0_BOM.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louis/Dropbox/Dev/Arduino/libraries/SmartMatrix3/extras/hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F272576-3275-8444-B8CB-5C78151C163D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13871860-92CC-414D-A6D5-CE209F449448}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10560" yWindow="460" windowWidth="23040" windowHeight="20540" tabRatio="966" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BOM(please fill in)" sheetId="2" r:id="rId1"/>
+    <sheet name="BOM" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="__Anonymous_Sheet_DB__1">#REF!</definedName>
     <definedName name="__Anonymous_Sheet_DB__2">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'BOM(please fill in)'!$A$3:$L$21</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">BOM!$A$3:$L$21</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
   <extLst>
@@ -431,10 +431,10 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -867,20 +867,20 @@
     </row>
     <row r="2" spans="1:12" s="6" customFormat="1">
       <c r="A2" s="7"/>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="17"/>
+      <c r="K2" s="18"/>
       <c r="L2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1241,7 @@
         <v>41</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="10" t="s">

</xml_diff>